<commit_message>
WIP: Added framework classes
</commit_message>
<xml_diff>
--- a/plan/PlanItSolution.xlsx
+++ b/plan/PlanItSolution.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ani_b\Documents\GitHub\planitSolution\plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suren\IdeaProjects\planitSolution\plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B703EF-7F93-413A-923B-1F12C241F8C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{582AB72B-09AF-477F-A138-91257F3B9458}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contact" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>Forename</t>
   </si>
@@ -43,6 +43,15 @@
   </si>
   <si>
     <t>email@test.com</t>
+  </si>
+  <si>
+    <t>PlanIt</t>
+  </si>
+  <si>
+    <t>Solution</t>
+  </si>
+  <si>
+    <t>Asd</t>
   </si>
 </sst>
 </file>
@@ -371,18 +380,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -399,12 +408,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
@@ -413,6 +422,23 @@
         <v>212345678</v>
       </c>
       <c r="E2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>123</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>